<commit_message>
Start on excel connection
</commit_message>
<xml_diff>
--- a/Database/analysisExcelConnection.xlsx
+++ b/Database/analysisExcelConnection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\tom\Documents\Visual Studio Code\Python Files\RocketReplayAnalysis\RocketReplayAnalysis\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tom\Documents\Programming Work\Python\RocketReplayAnalysis\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95865B78-30CE-4A82-B87D-4C64881256CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DCD70B-4F7B-46D5-8FD8-E1EBE9FA35B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D6C79A8F-9430-45D1-B395-B89EA2281A00}"/>
+    <workbookView xWindow="-7488" yWindow="4056" windowWidth="17280" windowHeight="9420" xr2:uid="{D6C79A8F-9430-45D1-B395-B89EA2281A00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,77 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>OneAgainstMany</t>
+  </si>
+  <si>
+    <t>Name:</t>
+  </si>
+  <si>
+    <t>Raw Value</t>
+  </si>
+  <si>
+    <t>Calculated Value</t>
+  </si>
+  <si>
+    <t>Percentage Of</t>
+  </si>
+  <si>
+    <t>Value Used:</t>
+  </si>
+  <si>
+    <t>Here</t>
+  </si>
+  <si>
+    <t>Index Pos</t>
+  </si>
+  <si>
+    <t>Index Length</t>
+  </si>
+  <si>
+    <t>Against Average</t>
+  </si>
+  <si>
+    <t>Against Median</t>
+  </si>
+  <si>
+    <t>Standard Deviations Away</t>
+  </si>
+  <si>
+    <t>Value Rarity</t>
+  </si>
+  <si>
+    <t>Relevancy</t>
+  </si>
+  <si>
+    <t>Relevancy * Against {Value}</t>
+  </si>
+  <si>
+    <t>Stat Mean</t>
+  </si>
+  <si>
+    <t>Stat Quartile 1</t>
+  </si>
+  <si>
+    <t>Stat Quartile 2</t>
+  </si>
+  <si>
+    <t>Stat Quartile 3</t>
+  </si>
+  <si>
+    <t>Stat Mode</t>
+  </si>
+  <si>
+    <t>Stat Standard Deviation</t>
+  </si>
+  <si>
+    <t>Stat Grouped Mode</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,14 +452,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AB9817-EB31-4467-A3EC-EE623E793CC5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="6" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Head to head Works
</commit_message>
<xml_diff>
--- a/Database/analysisExcelConnection.xlsx
+++ b/Database/analysisExcelConnection.xlsx
@@ -152,6 +152,24 @@
     <tableColumn id="23" name="AgainstStandardDeviation"/>
     <tableColumn id="24" name="StandardDeviationRelative"/>
     <tableColumn id="25" name="StandardDeviationDifferential"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="OutputAnalysis2" displayName="OutputAnalysis2" ref="AA1:AI7" headerRowCount="1">
+  <autoFilter ref="AA1:AI7"/>
+  <tableColumns count="9">
+    <tableColumn id="27" name="Name"/>
+    <tableColumn id="28" name="Value"/>
+    <tableColumn id="29" name="OurCount"/>
+    <tableColumn id="30" name="TheirCount"/>
+    <tableColumn id="31" name="OurSum"/>
+    <tableColumn id="32" name="TheirSum"/>
+    <tableColumn id="33" name="OurCount%"/>
+    <tableColumn id="34" name="TheirCount%"/>
+    <tableColumn id="35" name="Differential"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -458,7 +476,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y100"/>
+  <dimension ref="A1:AI100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:Y1048576"/>
@@ -592,6 +610,51 @@
           <t>StandardDeviationDifferential</t>
         </is>
       </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>OurCount</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>TheirCount</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>OurSum</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>TheirSum</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>OurCount%</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>TheirCount%</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>Differential</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -671,6 +734,37 @@
       <c r="Y2" t="n">
         <v>-12.75050557377676</v>
       </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>carName</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Fennec</t>
+        </is>
+      </c>
+      <c r="AC2" t="n">
+        <v>507</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>102</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>912</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>134</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.555921052631579</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.7611940298507462</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>-0.2052729772191673</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -750,6 +844,37 @@
       <c r="Y3" t="n">
         <v>-49.08754121646183</v>
       </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>carName</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Octane</t>
+        </is>
+      </c>
+      <c r="AC3" t="n">
+        <v>405</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>912</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>134</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0.4440789473684211</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0.2388059701492537</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0.2052729772191673</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -829,6 +954,35 @@
       <c r="Y4" t="n">
         <v>-31.49772710010906</v>
       </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>mvp</t>
+        </is>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>590</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>85</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>912</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>134</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0.6469298245614035</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0.6343283582089553</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0.01260146635244819</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -908,6 +1062,35 @@
       <c r="Y5" t="n">
         <v>-4.350970615793722</v>
       </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>mvp</t>
+        </is>
+      </c>
+      <c r="AB5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>322</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>49</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>912</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>134</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>0.3530701754385965</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0.3656716417910448</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>-0.0126014663524483</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -987,6 +1170,35 @@
       <c r="Y6" t="n">
         <v>-3.788451651286209</v>
       </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>scoredFirst</t>
+        </is>
+      </c>
+      <c r="AB6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>477</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>44</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>677</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>61</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0.7045790251107829</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0.7213114754098361</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>-0.01673245029905324</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1066,6 +1278,35 @@
       <c r="Y7" t="n">
         <v>38.96761959744398</v>
       </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>scoredFirst</t>
+        </is>
+      </c>
+      <c r="AB7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>200</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>17</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>677</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>61</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>0.2954209748892171</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>0.2786885245901639</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0.01673245029905324</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8416,8 +8657,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>